<commit_message>
2024-03-14 : Synchronize codes to the origin repository.
</commit_message>
<xml_diff>
--- a/TestData/Input/BookChartData.xlsx
+++ b/TestData/Input/BookChartData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cells-toolset\TestData\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EF6700-EC6F-4265-878C-FD6BE433199D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8FF2EE-75EB-4063-BA2C-61A57F6BA910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SaleTable" sheetId="7" r:id="rId1"/>
@@ -2112,6 +2112,9 @@
   <wetp:taskpane dockstate="right" visibility="1" width="350" row="7">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+  </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
@@ -2397,11 +2400,23 @@
 </we:webextension>
 </file>
 
+<file path=xl/webextensions/webextension2.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{EA0D50F4-EAD9-42F4-B2C2-BFC5B2971F52}">
+  <we:reference id="wa200006009" version="1.0.1.6" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA200006009" version="1.0.1.6" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3:G23"/>
     </sheetView>
   </sheetViews>
@@ -2793,8 +2808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385A9160-8778-46A2-83CC-743832A398DF}">
   <dimension ref="C6:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>